<commit_message>
New commit => 10/02/2021
</commit_message>
<xml_diff>
--- a/rrd/AppData/CaseAllocation.xlsx
+++ b/rrd/AppData/CaseAllocation.xlsx
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1842" uniqueCount="230">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1861" uniqueCount="240">
   <si>
     <t xml:space="preserve"> Status</t>
   </si>
@@ -742,6 +742,36 @@
   </si>
   <si>
     <t>00001268</t>
+  </si>
+  <si>
+    <t>00001299</t>
+  </si>
+  <si>
+    <t>00001313</t>
+  </si>
+  <si>
+    <t>00001314</t>
+  </si>
+  <si>
+    <t>00001315</t>
+  </si>
+  <si>
+    <t>00001325</t>
+  </si>
+  <si>
+    <t>00001326</t>
+  </si>
+  <si>
+    <t>00001327</t>
+  </si>
+  <si>
+    <t>00001345</t>
+  </si>
+  <si>
+    <t>00001346</t>
+  </si>
+  <si>
+    <t>00001347</t>
   </si>
 </sst>
 </file>
@@ -866,7 +896,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -901,6 +931,19 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1407,7 +1450,7 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE65995A-9C00-4D5B-8374-B6551AD156AA}">
-  <dimension ref="A1:V3"/>
+  <dimension ref="A1:Y3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="U2" sqref="U2"/>
@@ -1434,6 +1477,9 @@
     <col min="19" max="19" bestFit="true" customWidth="true" width="10.0" collapsed="true"/>
     <col min="21" max="21" bestFit="true" customWidth="true" width="7.85546875" collapsed="true"/>
     <col min="22" max="22" bestFit="true" customWidth="true" width="7.796875" collapsed="true"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" width="7.796875" collapsed="true"/>
+    <col min="24" max="24" bestFit="true" customWidth="true" width="7.796875" collapsed="true"/>
+    <col min="25" max="25" bestFit="true" customWidth="true" width="9.95703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.25">
@@ -1495,10 +1541,16 @@
       <c r="T1" s="19" t="s">
         <v>207</v>
       </c>
-      <c r="U1" s="20" t="s">
+      <c r="V1" t="s" s="30">
         <v>207</v>
       </c>
-      <c r="V1" t="s" s="30">
+      <c r="W1" t="s" s="33">
+        <v>207</v>
+      </c>
+      <c r="X1" t="s" s="34">
+        <v>207</v>
+      </c>
+      <c r="Y1" t="s" s="35">
         <v>207</v>
       </c>
     </row>
@@ -1557,6 +1609,15 @@
       <c r="V2" t="s">
         <v>228</v>
       </c>
+      <c r="W2" t="s">
+        <v>230</v>
+      </c>
+      <c r="X2" t="s">
+        <v>231</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>232</v>
+      </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" s="23" t="s">
@@ -1609,6 +1670,9 @@
       </c>
       <c r="Q3" s="27" t="s">
         <v>44</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>233</v>
       </c>
     </row>
   </sheetData>
@@ -2415,7 +2479,7 @@
         <v>24</v>
       </c>
       <c r="M2" s="15" t="s">
-        <v>163</v>
+        <v>43</v>
       </c>
       <c r="N2" t="s">
         <v>119</v>
@@ -2462,7 +2526,7 @@
         <v>24</v>
       </c>
       <c r="M3" s="15" t="s">
-        <v>163</v>
+        <v>43</v>
       </c>
       <c r="N3" t="s">
         <v>119</v>
@@ -2482,7 +2546,7 @@
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE2FD8E0-3822-4DAD-BA7D-12FF08028B70}">
-  <dimension ref="A1:R3"/>
+  <dimension ref="A1:T3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
@@ -2502,6 +2566,8 @@
     <col min="16" max="16" customWidth="true" width="28.140625" collapsed="true"/>
     <col min="17" max="17" customWidth="true" width="28.0" collapsed="true"/>
     <col min="18" max="18" bestFit="true" customWidth="true" width="7.796875" collapsed="true"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" width="7.796875" collapsed="true"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" width="9.95703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -2559,6 +2625,12 @@
       <c r="R1" t="s" s="31">
         <v>207</v>
       </c>
+      <c r="S1" t="s" s="40">
+        <v>207</v>
+      </c>
+      <c r="T1" t="s" s="41">
+        <v>207</v>
+      </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -2615,6 +2687,12 @@
       <c r="R2" t="s">
         <v>229</v>
       </c>
+      <c r="S2" t="s">
+        <v>234</v>
+      </c>
+      <c r="T2" t="s">
+        <v>235</v>
+      </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -2667,6 +2745,9 @@
       </c>
       <c r="Q3" s="10" t="s">
         <v>50</v>
+      </c>
+      <c r="T3" t="s">
+        <v>236</v>
       </c>
     </row>
   </sheetData>
@@ -4143,7 +4224,7 @@
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A4FECDA-E4E8-4EE5-8AD2-F1FF87F62289}">
-  <dimension ref="A1:S3"/>
+  <dimension ref="A1:T3"/>
   <sheetViews>
     <sheetView topLeftCell="K1" workbookViewId="0">
       <selection activeCell="Q2" sqref="Q2"/>
@@ -4161,7 +4242,9 @@
     <col min="15" max="15" customWidth="true" width="20.140625" collapsed="true"/>
     <col min="16" max="16" customWidth="true" width="30.140625" collapsed="true"/>
     <col min="17" max="17" customWidth="true" width="27.28515625" collapsed="true"/>
-    <col min="19" max="19" width="7.796875" customWidth="true" bestFit="true"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" width="7.796875" collapsed="true"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" width="7.796875" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" width="9.95703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
@@ -4220,6 +4303,9 @@
       <c r="S1" t="s" s="32">
         <v>207</v>
       </c>
+      <c r="T1" t="s" s="43">
+        <v>207</v>
+      </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -4275,6 +4361,9 @@
       </c>
       <c r="S2" t="s">
         <v>218</v>
+      </c>
+      <c r="T2" t="s">
+        <v>237</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">

</xml_diff>